<commit_message>
updated Literature Summary.xlsx to remove it from the sharepoint
</commit_message>
<xml_diff>
--- a/Literature Summary.xlsx
+++ b/Literature Summary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibamberg.sharepoint.com/sites/Plants-COIN/Freigegebene Dokumente/Literature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bstoj\OneDrive - Otto-Friedrich-Universität Bamberg\COINS-Plants\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{1CB0B603-D33D-4E2A-B0E2-BDE1031A2F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FE04515-38FA-4ADE-A2DC-023BC0D8996E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC3149C-AFE5-40D5-8840-0A9C5DD37C50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BFE8920-8E8F-49D3-AD34-8353FF9D97BB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{4BFE8920-8E8F-49D3-AD34-8353FF9D97BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Literature" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -766,7 +766,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,12 +826,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -848,7 +854,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -865,13 +871,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -882,6 +881,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -948,7 +966,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1246,23 +1264,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036B4B93-85E3-41A9-8837-3DF153365E90}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="6" width="57.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1"/>
-    <col min="8" max="16384" width="10.7109375" style="2"/>
+    <col min="6" max="6" width="57.1328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.73046875" style="1"/>
+    <col min="8" max="16384" width="10.73046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1285,7 +1303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="330">
+    <row r="2" spans="1:7" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1308,7 +1326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="409.5">
+    <row r="3" spans="1:7" ht="384.75" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1331,145 +1349,145 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="409.5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="356.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="240">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="199.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="345">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="409.5">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="285">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="242.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="409.5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" s="13" customFormat="1" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="300">
+    <row r="10" spans="1:7" ht="256.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1482,139 +1500,139 @@
       <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="210">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="409.5">
+    <row r="12" spans="1:7" ht="370.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="6" t="s">
         <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="300" customHeight="1">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="300" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="300" customHeight="1">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="300" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="300" customHeight="1">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="300" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="300" customHeight="1">
+    <row r="16" spans="1:7" ht="300" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1630,152 +1648,156 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="390">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="342" x14ac:dyDescent="0.45">
+      <c r="A17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="409.5">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="409.5">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="409.6">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="409.6">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="384.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="405">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="384.75" x14ac:dyDescent="0.45">
+      <c r="A22" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="255">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:7" s="13" customFormat="1" ht="242.25" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="10"/>
+      <c r="F23" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="10" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1809,21 +1831,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010098CA91A62DAC144DA5DC240DA8C05490" ma:contentTypeVersion="6" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="1795925c587e9bb095964e47c1b06dda">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f2a6442b-9777-4ae1-8e30-8e64f250bdab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="809afa856947c41e005a18140959bd86" ns2:_="">
     <xsd:import namespace="f2a6442b-9777-4ae1-8e30-8e64f250bdab"/>
@@ -1979,14 +1986,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA2EC7F8-437F-49C6-B05F-C5C8355F9327}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63659407-7D82-412E-A45F-2A79849A3B87}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f2a6442b-9777-4ae1-8e30-8e64f250bdab"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E6F3E65-A176-4C0B-92F2-758BB63E6699}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E6F3E65-A176-4C0B-92F2-758BB63E6699}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63659407-7D82-412E-A45F-2A79849A3B87}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA2EC7F8-437F-49C6-B05F-C5C8355F9327}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>